<commit_message>
added an example script, changes to csv parser
</commit_message>
<xml_diff>
--- a/data/snt_details.xlsx
+++ b/data/snt_details.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matty_gee/Dropbox/Projects/social_navigation_task/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="0" windowWidth="26880" windowHeight="26640" tabRatio="500"/>
+    <workbookView xWindow="15200" yWindow="460" windowWidth="28080" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="old_csv_for_logs" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
@@ -1293,7 +1298,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1303,11 +1308,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W230"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A207" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B214" sqref="B214"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="6" bestFit="1" customWidth="1"/>
@@ -1332,7 +1337,7 @@
     <col min="24" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="16" customFormat="1">
+    <row r="1" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1403,7 +1408,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="16" customFormat="1">
+    <row r="2" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -1454,7 +1459,7 @@
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
     </row>
-    <row r="3" spans="1:23" s="16" customFormat="1">
+    <row r="3" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>0</v>
       </c>
@@ -1505,7 +1510,7 @@
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
     </row>
-    <row r="4" spans="1:23" s="16" customFormat="1">
+    <row r="4" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>0</v>
       </c>
@@ -1556,7 +1561,7 @@
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
     </row>
-    <row r="5" spans="1:23" s="16" customFormat="1">
+    <row r="5" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>0</v>
       </c>
@@ -1607,7 +1612,7 @@
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
     </row>
-    <row r="6" spans="1:23" s="16" customFormat="1">
+    <row r="6" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>0</v>
       </c>
@@ -1658,7 +1663,7 @@
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
     </row>
-    <row r="7" spans="1:23" s="16" customFormat="1">
+    <row r="7" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>0</v>
       </c>
@@ -1709,7 +1714,7 @@
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -1753,7 +1758,7 @@
         <v>1.990000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>2</v>
       </c>
@@ -1797,7 +1802,7 @@
         <v>10.003</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>3</v>
       </c>
@@ -1838,7 +1843,7 @@
         <v>7.9990000000000023</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -1909,7 +1914,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>5</v>
       </c>
@@ -1950,7 +1955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -2021,7 +2026,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>7</v>
       </c>
@@ -2062,7 +2067,7 @@
         <v>8.0010000000000048</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>8</v>
       </c>
@@ -2133,7 +2138,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>9</v>
       </c>
@@ -2174,7 +2179,7 @@
         <v>8.0009999999999906</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>10</v>
       </c>
@@ -2216,7 +2221,7 @@
         <v>5.9880000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>11</v>
       </c>
@@ -2257,7 +2262,7 @@
         <v>2.00200000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>12</v>
       </c>
@@ -2328,7 +2333,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>13</v>
       </c>
@@ -2369,7 +2374,7 @@
         <v>3.9949999999999761</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>14</v>
       </c>
@@ -2411,7 +2416,7 @@
         <v>3.9960000000000089</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>15</v>
       </c>
@@ -2482,7 +2487,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>16</v>
       </c>
@@ -2524,7 +2529,7 @@
         <v>3.9920000000000191</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>17</v>
       </c>
@@ -2565,7 +2570,7 @@
         <v>5.9880000000000004</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>18</v>
       </c>
@@ -2636,7 +2641,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>19</v>
       </c>
@@ -2677,7 +2682,7 @@
         <v>3.9970000000000141</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>20</v>
       </c>
@@ -2719,7 +2724,7 @@
         <v>3.9889999999999759</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>21</v>
       </c>
@@ -2790,7 +2795,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>22</v>
       </c>
@@ -2861,7 +2866,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
         <v>23</v>
       </c>
@@ -2902,7 +2907,7 @@
         <v>4.0029999999999859</v>
       </c>
     </row>
-    <row r="31" spans="1:23">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>24</v>
       </c>
@@ -2944,7 +2949,7 @@
         <v>8.0010000000000048</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
         <v>25</v>
       </c>
@@ -2985,7 +2990,7 @@
         <v>3.9869999999999952</v>
       </c>
     </row>
-    <row r="33" spans="1:23">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>26</v>
       </c>
@@ -3056,7 +3061,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:23">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
         <v>27</v>
       </c>
@@ -3097,7 +3102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:23">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>28</v>
       </c>
@@ -3139,7 +3144,7 @@
         <v>4.0039999999999907</v>
       </c>
     </row>
-    <row r="36" spans="1:23">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
         <v>29</v>
       </c>
@@ -3210,7 +3215,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:23">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>30</v>
       </c>
@@ -3252,7 +3257,7 @@
         <v>5.9880000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:23">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
         <v>31</v>
       </c>
@@ -3293,7 +3298,7 @@
         <v>8.0009999999999764</v>
       </c>
     </row>
-    <row r="39" spans="1:23">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>32</v>
       </c>
@@ -3335,7 +3340,7 @@
         <v>3.98599999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:23">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
         <v>33</v>
       </c>
@@ -3376,7 +3381,7 @@
         <v>5.9880000000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:23">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>34</v>
       </c>
@@ -3418,7 +3423,7 @@
         <v>5.9889999999999759</v>
       </c>
     </row>
-    <row r="42" spans="1:23">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" s="6">
         <v>35</v>
       </c>
@@ -3459,7 +3464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:23">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>36</v>
       </c>
@@ -3501,7 +3506,7 @@
         <v>1.990999999999985</v>
       </c>
     </row>
-    <row r="44" spans="1:23">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="6">
         <v>37</v>
       </c>
@@ -3542,7 +3547,7 @@
         <v>2.00200000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:23">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>38</v>
       </c>
@@ -3613,7 +3618,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:23">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" s="6">
         <v>39</v>
       </c>
@@ -3654,7 +3659,7 @@
         <v>8.0010000000000332</v>
       </c>
     </row>
-    <row r="47" spans="1:23">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>40</v>
       </c>
@@ -3696,7 +3701,7 @@
         <v>4.0019999999999527</v>
       </c>
     </row>
-    <row r="48" spans="1:23">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" s="6">
         <v>41</v>
       </c>
@@ -3737,7 +3742,7 @@
         <v>8.0020000000000095</v>
       </c>
     </row>
-    <row r="49" spans="1:23">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>42</v>
       </c>
@@ -3779,7 +3784,7 @@
         <v>1.9900000000000091</v>
       </c>
     </row>
-    <row r="50" spans="1:23">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" s="6">
         <v>43</v>
       </c>
@@ -3820,7 +3825,7 @@
         <v>5.9880000000000004</v>
       </c>
     </row>
-    <row r="51" spans="1:23">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>44</v>
       </c>
@@ -3891,7 +3896,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:23">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" s="6">
         <v>45</v>
       </c>
@@ -3932,7 +3937,7 @@
         <v>9.9940000000000282</v>
       </c>
     </row>
-    <row r="53" spans="1:23">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>46</v>
       </c>
@@ -3974,7 +3979,7 @@
         <v>3.9869999999999659</v>
       </c>
     </row>
-    <row r="54" spans="1:23">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" s="6">
         <v>47</v>
       </c>
@@ -4015,7 +4020,7 @@
         <v>5.9880000000000004</v>
       </c>
     </row>
-    <row r="55" spans="1:23">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>48</v>
       </c>
@@ -4086,7 +4091,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:23">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56" s="6">
         <v>49</v>
       </c>
@@ -4127,7 +4132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:23">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>50</v>
       </c>
@@ -4169,7 +4174,7 @@
         <v>5.9880000000000004</v>
       </c>
     </row>
-    <row r="58" spans="1:23">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" s="6">
         <v>51</v>
       </c>
@@ -4240,7 +4245,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:23">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>52</v>
       </c>
@@ -4282,7 +4287,7 @@
         <v>3.9960000000000382</v>
       </c>
     </row>
-    <row r="60" spans="1:23">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" s="6">
         <v>53</v>
       </c>
@@ -4323,7 +4328,7 @@
         <v>4.0039999999999623</v>
       </c>
     </row>
-    <row r="61" spans="1:23">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>54</v>
       </c>
@@ -4390,7 +4395,7 @@
       <c r="V61" s="17"/>
       <c r="W61" s="17"/>
     </row>
-    <row r="62" spans="1:23">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62" s="6">
         <v>55</v>
       </c>
@@ -4431,7 +4436,7 @@
         <v>3.9939999999999709</v>
       </c>
     </row>
-    <row r="63" spans="1:23">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>56</v>
       </c>
@@ -4473,7 +4478,7 @@
         <v>1.9920000000000191</v>
       </c>
     </row>
-    <row r="64" spans="1:23">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64" s="6">
         <v>57</v>
       </c>
@@ -4540,7 +4545,7 @@
       <c r="V64" s="17"/>
       <c r="W64" s="17"/>
     </row>
-    <row r="65" spans="1:23">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>58</v>
       </c>
@@ -4582,7 +4587,7 @@
         <v>3.9960000000000382</v>
       </c>
     </row>
-    <row r="66" spans="1:23">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A66" s="6">
         <v>59</v>
       </c>
@@ -4623,7 +4628,7 @@
         <v>1.9900000000000091</v>
       </c>
     </row>
-    <row r="67" spans="1:23">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>60</v>
       </c>
@@ -4665,7 +4670,7 @@
         <v>1.990999999999985</v>
       </c>
     </row>
-    <row r="68" spans="1:23">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A68" s="6">
         <v>61</v>
       </c>
@@ -4706,7 +4711,7 @@
         <v>2.0039999999999618</v>
       </c>
     </row>
-    <row r="69" spans="1:23">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>62</v>
       </c>
@@ -4748,7 +4753,7 @@
         <v>9.992999999999995</v>
       </c>
     </row>
-    <row r="70" spans="1:23">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A70" s="6">
         <v>63</v>
       </c>
@@ -4819,7 +4824,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:23">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>64</v>
       </c>
@@ -4861,7 +4866,7 @@
         <v>5.9880000000000004</v>
       </c>
     </row>
-    <row r="72" spans="1:23">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A72" s="6">
         <v>65</v>
       </c>
@@ -4902,7 +4907,7 @@
         <v>6.0049999999999946</v>
       </c>
     </row>
-    <row r="73" spans="1:23">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>66</v>
       </c>
@@ -4973,7 +4978,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="74" spans="1:23">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A74" s="6">
         <v>67</v>
       </c>
@@ -5014,7 +5019,7 @@
         <v>3.988</v>
       </c>
     </row>
-    <row r="75" spans="1:23">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>68</v>
       </c>
@@ -5056,7 +5061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:23">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A76" s="6">
         <v>69</v>
       </c>
@@ -5097,7 +5102,7 @@
         <v>1.9889999999999759</v>
       </c>
     </row>
-    <row r="77" spans="1:23">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>70</v>
       </c>
@@ -5139,7 +5144,7 @@
         <v>3.9960000000000382</v>
       </c>
     </row>
-    <row r="78" spans="1:23">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A78" s="6">
         <v>71</v>
       </c>
@@ -5210,7 +5215,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="79" spans="1:23">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>72</v>
       </c>
@@ -5252,7 +5257,7 @@
         <v>3.995000000000005</v>
       </c>
     </row>
-    <row r="80" spans="1:23">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A80" s="6">
         <v>73</v>
       </c>
@@ -5293,7 +5298,7 @@
         <v>4.0030000000000427</v>
       </c>
     </row>
-    <row r="81" spans="1:23">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>74</v>
       </c>
@@ -5335,7 +5340,7 @@
         <v>3.995000000000005</v>
       </c>
     </row>
-    <row r="82" spans="1:23">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A82" s="6">
         <v>75</v>
       </c>
@@ -5376,7 +5381,7 @@
         <v>4.0039999999999054</v>
       </c>
     </row>
-    <row r="83" spans="1:23">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>76</v>
       </c>
@@ -5418,7 +5423,7 @@
         <v>3.9869999999999659</v>
       </c>
     </row>
-    <row r="84" spans="1:23">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A84" s="6">
         <v>77</v>
       </c>
@@ -5459,7 +5464,7 @@
         <v>3.9910000000000991</v>
       </c>
     </row>
-    <row r="85" spans="1:23">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>78</v>
       </c>
@@ -5501,7 +5506,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:23">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A86" s="6">
         <v>79</v>
       </c>
@@ -5542,7 +5547,7 @@
         <v>3.98700000000008</v>
       </c>
     </row>
-    <row r="87" spans="1:23">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>80</v>
       </c>
@@ -5613,7 +5618,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="88" spans="1:23">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A88" s="6">
         <v>81</v>
       </c>
@@ -5654,7 +5659,7 @@
         <v>4.0019999999999527</v>
       </c>
     </row>
-    <row r="89" spans="1:23">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>82</v>
       </c>
@@ -5725,7 +5730,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="90" spans="1:23">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A90" s="6">
         <v>83</v>
       </c>
@@ -5766,7 +5771,7 @@
         <v>8.0020000000000664</v>
       </c>
     </row>
-    <row r="91" spans="1:23">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>84</v>
       </c>
@@ -5808,7 +5813,7 @@
         <v>5.3659999999999846</v>
       </c>
     </row>
-    <row r="92" spans="1:23">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A92" s="6">
         <v>85</v>
       </c>
@@ -5879,7 +5884,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="93" spans="1:23">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>86</v>
       </c>
@@ -5921,7 +5926,7 @@
         <v>3.9919999999999618</v>
       </c>
     </row>
-    <row r="94" spans="1:23">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A94" s="6">
         <v>87</v>
       </c>
@@ -5962,7 +5967,7 @@
         <v>4.0030000000000427</v>
       </c>
     </row>
-    <row r="95" spans="1:23">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>88</v>
       </c>
@@ -6004,7 +6009,7 @@
         <v>3.990999999999985</v>
       </c>
     </row>
-    <row r="96" spans="1:23">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A96" s="6">
         <v>89</v>
       </c>
@@ -6075,7 +6080,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="97" spans="1:23">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>90</v>
       </c>
@@ -6117,7 +6122,7 @@
         <v>5.9880000000000564</v>
       </c>
     </row>
-    <row r="98" spans="1:23">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A98" s="6">
         <v>91</v>
       </c>
@@ -6188,7 +6193,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="99" spans="1:23">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>92</v>
       </c>
@@ -6230,7 +6235,7 @@
         <v>5.9890000000000327</v>
       </c>
     </row>
-    <row r="100" spans="1:23">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A100" s="6">
         <v>93</v>
       </c>
@@ -6271,7 +6276,7 @@
         <v>3.98599999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:23">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>94</v>
       </c>
@@ -6342,7 +6347,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:23">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A102" s="6">
         <v>95</v>
       </c>
@@ -6383,7 +6388,7 @@
         <v>5.98700000000008</v>
       </c>
     </row>
-    <row r="103" spans="1:23">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>96</v>
       </c>
@@ -6454,7 +6459,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="104" spans="1:23">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A104" s="6">
         <v>97</v>
       </c>
@@ -6495,7 +6500,7 @@
         <v>3.9860000000001041</v>
       </c>
     </row>
-    <row r="105" spans="1:23">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>98</v>
       </c>
@@ -6537,7 +6542,7 @@
         <v>3.9930000000000518</v>
       </c>
     </row>
-    <row r="106" spans="1:23">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A106" s="6">
         <v>99</v>
       </c>
@@ -6578,7 +6583,7 @@
         <v>1.994000000000028</v>
       </c>
     </row>
-    <row r="107" spans="1:23">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>100</v>
       </c>
@@ -6620,7 +6625,7 @@
         <v>3.9930000000000518</v>
       </c>
     </row>
-    <row r="108" spans="1:23">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A108" s="6">
         <v>101</v>
       </c>
@@ -6691,7 +6696,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="109" spans="1:23">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>102</v>
       </c>
@@ -6733,7 +6738,7 @@
         <v>3.9869999999999659</v>
       </c>
     </row>
-    <row r="110" spans="1:23">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A110" s="6">
         <v>103</v>
       </c>
@@ -6774,7 +6779,7 @@
         <v>3.990999999999985</v>
       </c>
     </row>
-    <row r="111" spans="1:23">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>104</v>
       </c>
@@ -6816,7 +6821,7 @@
         <v>9.9880000000000564</v>
       </c>
     </row>
-    <row r="112" spans="1:23">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A112" s="6">
         <v>105</v>
       </c>
@@ -6857,7 +6862,7 @@
         <v>7.9959999999999809</v>
       </c>
     </row>
-    <row r="113" spans="1:23">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>106</v>
       </c>
@@ -6928,7 +6933,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="114" spans="1:23">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A114" s="6">
         <v>107</v>
       </c>
@@ -6969,7 +6974,7 @@
         <v>5.9880000000000564</v>
       </c>
     </row>
-    <row r="115" spans="1:23">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>108</v>
       </c>
@@ -7011,7 +7016,7 @@
         <v>5.9879999999999427</v>
       </c>
     </row>
-    <row r="116" spans="1:23">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A116" s="6">
         <v>109</v>
       </c>
@@ -7052,7 +7057,7 @@
         <v>3.9929999999999382</v>
       </c>
     </row>
-    <row r="117" spans="1:23">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>110</v>
       </c>
@@ -7094,7 +7099,7 @@
         <v>3.995000000000005</v>
       </c>
     </row>
-    <row r="118" spans="1:23">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A118" s="6">
         <v>111</v>
       </c>
@@ -7165,7 +7170,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="119" spans="1:23">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>112</v>
       </c>
@@ -7207,7 +7212,7 @@
         <v>5.9879999999999427</v>
       </c>
     </row>
-    <row r="120" spans="1:23">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A120" s="6">
         <v>113</v>
       </c>
@@ -7248,7 +7253,7 @@
         <v>4.0019999999999527</v>
       </c>
     </row>
-    <row r="121" spans="1:23">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>114</v>
       </c>
@@ -7290,7 +7295,7 @@
         <v>1.992000000000075</v>
       </c>
     </row>
-    <row r="122" spans="1:23">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A122" s="6">
         <v>115</v>
       </c>
@@ -7331,7 +7336,7 @@
         <v>2.0020000000000659</v>
       </c>
     </row>
-    <row r="123" spans="1:23">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>116</v>
       </c>
@@ -7373,7 +7378,7 @@
         <v>1.9869999999999659</v>
       </c>
     </row>
-    <row r="124" spans="1:23">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A124" s="6">
         <v>117</v>
       </c>
@@ -7414,7 +7419,7 @@
         <v>3.990999999999985</v>
       </c>
     </row>
-    <row r="125" spans="1:23">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>118</v>
       </c>
@@ -7456,7 +7461,7 @@
         <v>3.9930000000000518</v>
       </c>
     </row>
-    <row r="126" spans="1:23">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A126" s="6">
         <v>119</v>
       </c>
@@ -7497,7 +7502,7 @@
         <v>3.995000000000005</v>
       </c>
     </row>
-    <row r="127" spans="1:23">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>120</v>
       </c>
@@ -7539,7 +7544,7 @@
         <v>3.9959999999999809</v>
       </c>
     </row>
-    <row r="128" spans="1:23">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A128" s="6">
         <v>121</v>
       </c>
@@ -7580,7 +7585,7 @@
         <v>4.0030000000000427</v>
       </c>
     </row>
-    <row r="129" spans="1:23">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>122</v>
       </c>
@@ -7622,7 +7627,7 @@
         <v>3.9869999999999659</v>
       </c>
     </row>
-    <row r="130" spans="1:23">
+    <row r="130" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A130" s="6">
         <v>123</v>
       </c>
@@ -7693,7 +7698,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="131" spans="1:23">
+    <row r="131" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>124</v>
       </c>
@@ -7735,7 +7740,7 @@
         <v>3.996000000000095</v>
       </c>
     </row>
-    <row r="132" spans="1:23">
+    <row r="132" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A132" s="6">
         <v>125</v>
       </c>
@@ -7776,7 +7781,7 @@
         <v>4.0019999999999527</v>
       </c>
     </row>
-    <row r="133" spans="1:23">
+    <row r="133" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>126</v>
       </c>
@@ -7818,7 +7823,7 @@
         <v>5.9879999999999427</v>
       </c>
     </row>
-    <row r="134" spans="1:23">
+    <row r="134" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A134" s="6">
         <v>127</v>
       </c>
@@ -7889,7 +7894,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="135" spans="1:23">
+    <row r="135" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>128</v>
       </c>
@@ -7931,7 +7936,7 @@
         <v>3.9850000000000141</v>
       </c>
     </row>
-    <row r="136" spans="1:23">
+    <row r="136" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A136" s="6">
         <v>129</v>
       </c>
@@ -7972,7 +7977,7 @@
         <v>3.9969999999999568</v>
       </c>
     </row>
-    <row r="137" spans="1:23">
+    <row r="137" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>130</v>
       </c>
@@ -8043,7 +8048,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="138" spans="1:23">
+    <row r="138" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A138" s="6">
         <v>131</v>
       </c>
@@ -8084,7 +8089,7 @@
         <v>7.9890000000000327</v>
       </c>
     </row>
-    <row r="139" spans="1:23">
+    <row r="139" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>132</v>
       </c>
@@ -8126,7 +8131,7 @@
         <v>8.0030000000000427</v>
       </c>
     </row>
-    <row r="140" spans="1:23">
+    <row r="140" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A140" s="6">
         <v>133</v>
       </c>
@@ -8197,7 +8202,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="141" spans="1:23">
+    <row r="141" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>134</v>
       </c>
@@ -8239,7 +8244,7 @@
         <v>3.9959999999999809</v>
       </c>
     </row>
-    <row r="142" spans="1:23">
+    <row r="142" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A142" s="6">
         <v>135</v>
       </c>
@@ -8310,7 +8315,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="143" spans="1:23">
+    <row r="143" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>136</v>
       </c>
@@ -8352,7 +8357,7 @@
         <v>4.0020000000000664</v>
       </c>
     </row>
-    <row r="144" spans="1:23">
+    <row r="144" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A144" s="6">
         <v>137</v>
       </c>
@@ -8393,7 +8398,7 @@
         <v>1.990999999999985</v>
       </c>
     </row>
-    <row r="145" spans="1:23">
+    <row r="145" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>138</v>
       </c>
@@ -8435,7 +8440,7 @@
         <v>3.9959999999999809</v>
       </c>
     </row>
-    <row r="146" spans="1:23">
+    <row r="146" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A146" s="6">
         <v>139</v>
       </c>
@@ -8506,7 +8511,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="147" spans="1:23">
+    <row r="147" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>140</v>
       </c>
@@ -8548,7 +8553,7 @@
         <v>3.98599999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:23">
+    <row r="148" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A148" s="6">
         <v>141</v>
       </c>
@@ -8589,7 +8594,7 @@
         <v>3.992000000000075</v>
       </c>
     </row>
-    <row r="149" spans="1:23">
+    <row r="149" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>142</v>
       </c>
@@ -8656,7 +8661,7 @@
       <c r="V149" s="17"/>
       <c r="W149" s="17"/>
     </row>
-    <row r="150" spans="1:23">
+    <row r="150" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A150" s="6">
         <v>143</v>
       </c>
@@ -8697,7 +8702,7 @@
         <v>5.9889999999999191</v>
       </c>
     </row>
-    <row r="151" spans="1:23">
+    <row r="151" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>144</v>
       </c>
@@ -8739,7 +8744,7 @@
         <v>4.0040000000000191</v>
       </c>
     </row>
-    <row r="152" spans="1:23">
+    <row r="152" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A152" s="6">
         <v>145</v>
       </c>
@@ -8810,7 +8815,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="153" spans="1:23">
+    <row r="153" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>146</v>
       </c>
@@ -8852,7 +8857,7 @@
         <v>3.9869999999999659</v>
       </c>
     </row>
-    <row r="154" spans="1:23">
+    <row r="154" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A154" s="6">
         <v>147</v>
       </c>
@@ -8893,7 +8898,7 @@
         <v>3.992000000000075</v>
       </c>
     </row>
-    <row r="155" spans="1:23">
+    <row r="155" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>148</v>
       </c>
@@ -8964,7 +8969,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="156" spans="1:23">
+    <row r="156" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A156" s="6">
         <v>149</v>
       </c>
@@ -9005,7 +9010,7 @@
         <v>5.9890000000000327</v>
       </c>
     </row>
-    <row r="157" spans="1:23">
+    <row r="157" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>150</v>
       </c>
@@ -9076,7 +9081,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="158" spans="1:23">
+    <row r="158" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A158" s="6">
         <v>151</v>
       </c>
@@ -9117,7 +9122,7 @@
         <v>3.9949999999998909</v>
       </c>
     </row>
-    <row r="159" spans="1:23">
+    <row r="159" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>152</v>
       </c>
@@ -9159,7 +9164,7 @@
         <v>5.987999999999829</v>
       </c>
     </row>
-    <row r="160" spans="1:23">
+    <row r="160" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A160" s="6">
         <v>153</v>
       </c>
@@ -9230,7 +9235,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="161" spans="1:23">
+    <row r="161" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>154</v>
       </c>
@@ -9272,7 +9277,7 @@
         <v>3.996000000000095</v>
       </c>
     </row>
-    <row r="162" spans="1:23">
+    <row r="162" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A162" s="6">
         <v>155</v>
       </c>
@@ -9313,7 +9318,7 @@
         <v>4.0019999999999527</v>
       </c>
     </row>
-    <row r="163" spans="1:23">
+    <row r="163" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>156</v>
       </c>
@@ -9384,7 +9389,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="164" spans="1:23">
+    <row r="164" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A164" s="6">
         <v>157</v>
       </c>
@@ -9425,7 +9430,7 @@
         <v>3.9949999999998909</v>
       </c>
     </row>
-    <row r="165" spans="1:23">
+    <row r="165" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>158</v>
       </c>
@@ -9496,7 +9501,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="166" spans="1:23">
+    <row r="166" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A166" s="6">
         <v>159</v>
       </c>
@@ -9537,7 +9542,7 @@
         <v>5.9949999999998909</v>
       </c>
     </row>
-    <row r="167" spans="1:23">
+    <row r="167" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>160</v>
       </c>
@@ -9579,7 +9584,7 @@
         <v>4.0040000000001328</v>
       </c>
     </row>
-    <row r="168" spans="1:23">
+    <row r="168" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A168" s="6">
         <v>161</v>
       </c>
@@ -9650,7 +9655,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="169" spans="1:23">
+    <row r="169" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>162</v>
       </c>
@@ -9692,7 +9697,7 @@
         <v>3.9859999999998759</v>
       </c>
     </row>
-    <row r="170" spans="1:23">
+    <row r="170" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A170" s="6">
         <v>163</v>
       </c>
@@ -9763,7 +9768,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="171" spans="1:23">
+    <row r="171" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>164</v>
       </c>
@@ -9805,7 +9810,7 @@
         <v>3.996000000000095</v>
       </c>
     </row>
-    <row r="172" spans="1:23">
+    <row r="172" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A172" s="6">
         <v>165</v>
       </c>
@@ -9876,7 +9881,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="173" spans="1:23">
+    <row r="173" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>166</v>
       </c>
@@ -9918,7 +9923,7 @@
         <v>3.9859999999998759</v>
       </c>
     </row>
-    <row r="174" spans="1:23">
+    <row r="174" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A174" s="6">
         <v>167</v>
       </c>
@@ -9959,7 +9964,7 @@
         <v>3.9919999999999618</v>
       </c>
     </row>
-    <row r="175" spans="1:23">
+    <row r="175" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>168</v>
       </c>
@@ -10030,7 +10035,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="176" spans="1:23">
+    <row r="176" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A176" s="6">
         <v>169</v>
       </c>
@@ -10071,7 +10076,7 @@
         <v>5.9890000000000327</v>
       </c>
     </row>
-    <row r="177" spans="1:23">
+    <row r="177" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>170</v>
       </c>
@@ -10113,7 +10118,7 @@
         <v>4.0040000000001328</v>
       </c>
     </row>
-    <row r="178" spans="1:23">
+    <row r="178" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A178" s="6">
         <v>171</v>
       </c>
@@ -10154,7 +10159,7 @@
         <v>3.9949999999998909</v>
       </c>
     </row>
-    <row r="179" spans="1:23">
+    <row r="179" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>172</v>
       </c>
@@ -10196,7 +10201,7 @@
         <v>4.0019999999999527</v>
       </c>
     </row>
-    <row r="180" spans="1:23">
+    <row r="180" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A180" s="6">
         <v>173</v>
       </c>
@@ -10267,7 +10272,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="181" spans="1:23">
+    <row r="181" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>174</v>
       </c>
@@ -10338,7 +10343,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="182" spans="1:23">
+    <row r="182" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A182" s="6">
         <v>175</v>
       </c>
@@ -10379,7 +10384,7 @@
         <v>5.98700000000008</v>
       </c>
     </row>
-    <row r="183" spans="1:23">
+    <row r="183" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>176</v>
       </c>
@@ -10421,7 +10426,7 @@
         <v>4.0039999999999054</v>
       </c>
     </row>
-    <row r="184" spans="1:23">
+    <row r="184" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A184" s="6">
         <v>177</v>
       </c>
@@ -10492,7 +10497,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="185" spans="1:23">
+    <row r="185" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>178</v>
       </c>
@@ -10534,7 +10539,7 @@
         <v>3.996000000000095</v>
       </c>
     </row>
-    <row r="186" spans="1:23">
+    <row r="186" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A186" s="6">
         <v>179</v>
       </c>
@@ -10575,7 +10580,7 @@
         <v>3.98700000000008</v>
       </c>
     </row>
-    <row r="187" spans="1:23">
+    <row r="187" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>180</v>
       </c>
@@ -10617,7 +10622,7 @@
         <v>3.9929999999999382</v>
       </c>
     </row>
-    <row r="188" spans="1:23">
+    <row r="188" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A188" s="6">
         <v>181</v>
       </c>
@@ -10688,7 +10693,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="189" spans="1:23">
+    <row r="189" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>182</v>
       </c>
@@ -10730,7 +10735,7 @@
         <v>5.9890000000000327</v>
       </c>
     </row>
-    <row r="190" spans="1:23">
+    <row r="190" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A190" s="6">
         <v>183</v>
       </c>
@@ -10771,7 +10776,7 @@
         <v>5.98700000000008</v>
       </c>
     </row>
-    <row r="191" spans="1:23">
+    <row r="191" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>184</v>
       </c>
@@ -10842,7 +10847,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="192" spans="1:23">
+    <row r="192" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A192" s="6">
         <v>185</v>
       </c>
@@ -10883,7 +10888,7 @@
         <v>7.9900000000000091</v>
       </c>
     </row>
-    <row r="193" spans="1:23">
+    <row r="193" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>186</v>
       </c>
@@ -10925,7 +10930,7 @@
         <v>5.987999999999829</v>
       </c>
     </row>
-    <row r="194" spans="1:23">
+    <row r="194" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A194" s="6">
         <v>187</v>
       </c>
@@ -10996,7 +11001,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="195" spans="1:23">
+    <row r="195" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>188</v>
       </c>
@@ -11038,7 +11043,7 @@
         <v>5.987999999999829</v>
       </c>
     </row>
-    <row r="196" spans="1:23">
+    <row r="196" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A196" s="6">
         <v>189</v>
       </c>
@@ -11079,7 +11084,7 @@
         <v>3.9869999999998531</v>
       </c>
     </row>
-    <row r="197" spans="1:23">
+    <row r="197" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>190</v>
       </c>
@@ -11150,7 +11155,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="198" spans="1:23">
+    <row r="198" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A198" s="6">
         <v>191</v>
       </c>
@@ -11191,7 +11196,7 @@
         <v>8.0009999999999764</v>
       </c>
     </row>
-    <row r="199" spans="1:23">
+    <row r="199" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>192</v>
       </c>
@@ -11233,7 +11238,7 @@
         <v>5.9890000000000327</v>
       </c>
     </row>
-    <row r="200" spans="1:23">
+    <row r="200" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A200" s="6">
         <v>193</v>
       </c>
@@ -11304,7 +11309,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="201" spans="1:23">
+    <row r="201" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>194</v>
       </c>
@@ -11346,7 +11351,7 @@
         <v>4.0040000000001328</v>
       </c>
     </row>
-    <row r="202" spans="1:23">
+    <row r="202" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A202" s="6">
         <v>195</v>
       </c>
@@ -11417,7 +11422,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="203" spans="1:23">
+    <row r="203" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>196</v>
       </c>
@@ -11459,7 +11464,7 @@
         <v>9.9929999999999382</v>
       </c>
     </row>
-    <row r="204" spans="1:23">
+    <row r="204" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A204" s="6">
         <v>197</v>
       </c>
@@ -11530,7 +11535,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="205" spans="1:23">
+    <row r="205" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>198</v>
       </c>
@@ -11572,7 +11577,7 @@
         <v>5.9880000000000564</v>
       </c>
     </row>
-    <row r="206" spans="1:23">
+    <row r="206" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A206" s="6">
         <v>199</v>
       </c>
@@ -11643,7 +11648,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="207" spans="1:23">
+    <row r="207" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>200</v>
       </c>
@@ -11685,7 +11690,7 @@
         <v>3.996000000000095</v>
       </c>
     </row>
-    <row r="208" spans="1:23">
+    <row r="208" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A208" s="6">
         <v>201</v>
       </c>
@@ -11756,7 +11761,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="209" spans="1:23">
+    <row r="209" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>202</v>
       </c>
@@ -11798,7 +11803,7 @@
         <v>9.9859999999998763</v>
       </c>
     </row>
-    <row r="210" spans="1:23">
+    <row r="210" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A210" s="6">
         <v>203</v>
       </c>
@@ -11869,7 +11874,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="211" spans="1:23">
+    <row r="211" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>204</v>
       </c>
@@ -11911,7 +11916,7 @@
         <v>4.0040000000001328</v>
       </c>
     </row>
-    <row r="212" spans="1:23">
+    <row r="212" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A212" s="6">
         <v>205</v>
       </c>
@@ -11952,7 +11957,7 @@
         <v>5.9890000000000327</v>
       </c>
     </row>
-    <row r="213" spans="1:23">
+    <row r="213" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>206</v>
       </c>
@@ -12023,7 +12028,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="214" spans="1:23">
+    <row r="214" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A214" s="6">
         <v>207</v>
       </c>
@@ -12064,7 +12069,7 @@
         <v>7.9969999999998436</v>
       </c>
     </row>
-    <row r="215" spans="1:23">
+    <row r="215" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>208</v>
       </c>
@@ -12135,7 +12140,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="216" spans="1:23">
+    <row r="216" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A216" s="6">
         <v>209</v>
       </c>
@@ -12176,7 +12181,7 @@
         <v>4.0019999999999527</v>
       </c>
     </row>
-    <row r="217" spans="1:23">
+    <row r="217" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>210</v>
       </c>
@@ -12218,7 +12223,7 @@
         <v>3.9869999999998531</v>
       </c>
     </row>
-    <row r="218" spans="1:23">
+    <row r="218" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A218" s="6">
         <v>211</v>
       </c>
@@ -12289,7 +12294,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="219" spans="1:23">
+    <row r="219" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>212</v>
       </c>
@@ -12331,7 +12336,7 @@
         <v>4.0040000000001328</v>
       </c>
     </row>
-    <row r="220" spans="1:23">
+    <row r="220" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A220" s="6">
         <v>213</v>
       </c>
@@ -12372,7 +12377,7 @@
         <v>3.993999999999915</v>
       </c>
     </row>
-    <row r="221" spans="1:23">
+    <row r="221" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>214</v>
       </c>
@@ -12414,7 +12419,7 @@
         <v>5.9969999999998436</v>
       </c>
     </row>
-    <row r="222" spans="1:23">
+    <row r="222" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A222" s="6">
         <v>215</v>
       </c>
@@ -12485,7 +12490,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="223" spans="1:23">
+    <row r="223" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A223" s="6">
         <v>216</v>
       </c>
@@ -12526,7 +12531,7 @@
         <v>5.9890000000000327</v>
       </c>
     </row>
-    <row r="224" spans="1:23">
+    <row r="224" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A224" s="6">
         <v>217</v>
       </c>
@@ -12562,14 +12567,14 @@
         <v>1528.097</v>
       </c>
       <c r="P224" s="10">
-        <f>O224+6</f>
+        <f t="shared" ref="P224:P230" si="0">O224+6</f>
         <v>1534.097</v>
       </c>
       <c r="Q224" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="225" spans="1:17">
+    <row r="225" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A225" s="5">
         <v>999</v>
       </c>
@@ -12608,14 +12613,14 @@
         <v>1528.097</v>
       </c>
       <c r="P225" s="10">
-        <f>O225+6</f>
+        <f t="shared" si="0"/>
         <v>1534.097</v>
       </c>
       <c r="Q225" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="226" spans="1:17">
+    <row r="226" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A226" s="5">
         <v>999</v>
       </c>
@@ -12655,14 +12660,14 @@
         <v>1534.097</v>
       </c>
       <c r="P226" s="10">
-        <f>O226+6</f>
+        <f t="shared" si="0"/>
         <v>1540.097</v>
       </c>
       <c r="Q226" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="227" spans="1:17">
+    <row r="227" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A227" s="5">
         <v>999</v>
       </c>
@@ -12702,14 +12707,14 @@
         <v>1540.097</v>
       </c>
       <c r="P227" s="10">
-        <f>O227+6</f>
+        <f t="shared" si="0"/>
         <v>1546.097</v>
       </c>
       <c r="Q227" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="228" spans="1:17">
+    <row r="228" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A228" s="5">
         <v>999</v>
       </c>
@@ -12749,14 +12754,14 @@
         <v>1546.097</v>
       </c>
       <c r="P228" s="10">
-        <f>O228+6</f>
+        <f t="shared" si="0"/>
         <v>1552.097</v>
       </c>
       <c r="Q228" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="229" spans="1:17">
+    <row r="229" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A229" s="5">
         <v>999</v>
       </c>
@@ -12796,14 +12801,14 @@
         <v>1552.097</v>
       </c>
       <c r="P229" s="10">
-        <f>O229+6</f>
+        <f t="shared" si="0"/>
         <v>1558.097</v>
       </c>
       <c r="Q229" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="230" spans="1:17">
+    <row r="230" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A230" s="5">
         <v>999</v>
       </c>
@@ -12843,7 +12848,7 @@
         <v>1558.097</v>
       </c>
       <c r="P230" s="10">
-        <f>O230+6</f>
+        <f t="shared" si="0"/>
         <v>1564.097</v>
       </c>
       <c r="Q230" s="5">
@@ -12856,11 +12861,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -12872,9 +12872,9 @@
       <selection activeCell="F2" sqref="F2:F64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>172</v>
       </c>
@@ -12894,7 +12894,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -12914,7 +12914,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -12934,7 +12934,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -12954,7 +12954,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -12974,7 +12974,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -12994,7 +12994,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -13014,7 +13014,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -13034,7 +13034,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -13054,7 +13054,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -13074,7 +13074,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -13094,7 +13094,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -13114,7 +13114,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -13134,7 +13134,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -13154,7 +13154,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -13174,7 +13174,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -13194,7 +13194,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -13214,7 +13214,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -13234,7 +13234,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -13254,7 +13254,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -13274,7 +13274,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -13294,7 +13294,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -13314,7 +13314,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -13334,7 +13334,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -13354,7 +13354,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -13374,7 +13374,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -13394,7 +13394,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -13414,7 +13414,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -13434,7 +13434,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -13454,7 +13454,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -13474,7 +13474,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -13494,7 +13494,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -13514,7 +13514,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -13534,7 +13534,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -13554,7 +13554,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -13574,7 +13574,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -13594,7 +13594,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -13614,7 +13614,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -13634,7 +13634,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -13654,7 +13654,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -13674,7 +13674,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -13694,7 +13694,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -13714,7 +13714,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -13734,7 +13734,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -13754,7 +13754,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -13774,7 +13774,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -13794,7 +13794,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -13814,7 +13814,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -13834,7 +13834,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -13854,7 +13854,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -13874,7 +13874,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -13894,7 +13894,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -13914,7 +13914,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -13934,7 +13934,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -13954,7 +13954,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -13974,7 +13974,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -13994,7 +13994,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -14014,7 +14014,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -14034,7 +14034,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -14054,7 +14054,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -14074,7 +14074,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -14094,7 +14094,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -14114,7 +14114,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -14134,7 +14134,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -14157,10 +14157,5 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working on new compute behavior class
</commit_message>
<xml_diff>
--- a/data/snt_details.xlsx
+++ b/data/snt_details.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matty_gee/Dropbox/Projects/social_navigation_task/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matty_gee/Dropbox/Projects/social_navigation_analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15200" yWindow="460" windowWidth="28080" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="5520" yWindow="460" windowWidth="28080" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1308,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B214" sqref="B214"/>
+    <sheetView tabSelected="1" topLeftCell="E132" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="I148" sqref="I148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1847,7 +1847,7 @@
       <c r="A11" s="1">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="15" t="s">
         <v>179</v>
       </c>
       <c r="C11" s="6">
@@ -1959,7 +1959,7 @@
       <c r="A13" s="1">
         <v>6</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="15" t="s">
         <v>180</v>
       </c>
       <c r="C13" s="6">
@@ -2071,7 +2071,7 @@
       <c r="A15" s="1">
         <v>8</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="15" t="s">
         <v>181</v>
       </c>
       <c r="C15" s="6">
@@ -2266,7 +2266,7 @@
       <c r="A19" s="1">
         <v>12</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="15" t="s">
         <v>182</v>
       </c>
       <c r="C19" s="2">
@@ -2420,7 +2420,7 @@
       <c r="A22" s="6">
         <v>15</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="15" t="s">
         <v>183</v>
       </c>
       <c r="C22" s="2">
@@ -2574,7 +2574,7 @@
       <c r="A25" s="1">
         <v>18</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="15" t="s">
         <v>184</v>
       </c>
       <c r="C25" s="2">
@@ -2728,7 +2728,7 @@
       <c r="A28" s="6">
         <v>21</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="15" t="s">
         <v>185</v>
       </c>
       <c r="C28" s="2">
@@ -2799,7 +2799,7 @@
       <c r="A29" s="1">
         <v>22</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="15" t="s">
         <v>186</v>
       </c>
       <c r="C29" s="2">
@@ -2994,7 +2994,7 @@
       <c r="A33" s="1">
         <v>26</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="15" t="s">
         <v>187</v>
       </c>
       <c r="C33" s="2">
@@ -3148,7 +3148,7 @@
       <c r="A36" s="6">
         <v>29</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="15" t="s">
         <v>188</v>
       </c>
       <c r="C36" s="6">
@@ -3551,7 +3551,7 @@
       <c r="A45" s="1">
         <v>38</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="15" t="s">
         <v>189</v>
       </c>
       <c r="C45" s="6">
@@ -3829,7 +3829,7 @@
       <c r="A51" s="1">
         <v>44</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="15" t="s">
         <v>190</v>
       </c>
       <c r="C51" s="6">
@@ -4024,7 +4024,7 @@
       <c r="A55" s="1">
         <v>48</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="15" t="s">
         <v>191</v>
       </c>
       <c r="C55" s="6">
@@ -4178,7 +4178,7 @@
       <c r="A58" s="6">
         <v>51</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="15" t="s">
         <v>192</v>
       </c>
       <c r="C58" s="6">
@@ -4332,7 +4332,7 @@
       <c r="A61" s="1">
         <v>54</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="15" t="s">
         <v>193</v>
       </c>
       <c r="C61" s="6">
@@ -4354,7 +4354,7 @@
         <v>14</v>
       </c>
       <c r="I61" s="6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J61" s="15">
         <v>0</v>
@@ -4482,7 +4482,7 @@
       <c r="A64" s="6">
         <v>57</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="15" t="s">
         <v>194</v>
       </c>
       <c r="C64" s="6">
@@ -4504,7 +4504,7 @@
         <v>14</v>
       </c>
       <c r="I64" s="6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J64" s="15">
         <v>0</v>
@@ -4757,7 +4757,7 @@
       <c r="A70" s="6">
         <v>63</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="15" t="s">
         <v>195</v>
       </c>
       <c r="C70" s="6">
@@ -4911,7 +4911,7 @@
       <c r="A73" s="1">
         <v>66</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="15" t="s">
         <v>196</v>
       </c>
       <c r="C73" s="6">
@@ -5148,7 +5148,7 @@
       <c r="A78" s="6">
         <v>71</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="15" t="s">
         <v>197</v>
       </c>
       <c r="C78" s="6">
@@ -5551,7 +5551,7 @@
       <c r="A87" s="1">
         <v>80</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="15" t="s">
         <v>198</v>
       </c>
       <c r="C87" s="6">
@@ -5663,7 +5663,7 @@
       <c r="A89" s="1">
         <v>82</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="15" t="s">
         <v>199</v>
       </c>
       <c r="C89" s="6">
@@ -5817,7 +5817,7 @@
       <c r="A92" s="6">
         <v>85</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="15" t="s">
         <v>200</v>
       </c>
       <c r="C92" s="6">
@@ -6013,7 +6013,7 @@
       <c r="A96" s="6">
         <v>89</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="15" t="s">
         <v>201</v>
       </c>
       <c r="C96" s="2">
@@ -6126,7 +6126,7 @@
       <c r="A98" s="6">
         <v>91</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="15" t="s">
         <v>202</v>
       </c>
       <c r="C98" s="2">
@@ -6280,7 +6280,7 @@
       <c r="A101" s="1">
         <v>94</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="15" t="s">
         <v>203</v>
       </c>
       <c r="C101" s="2">
@@ -6392,7 +6392,7 @@
       <c r="A103" s="1">
         <v>96</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="15" t="s">
         <v>204</v>
       </c>
       <c r="C103" s="6">
@@ -6629,7 +6629,7 @@
       <c r="A108" s="6">
         <v>101</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="15" t="s">
         <v>205</v>
       </c>
       <c r="C108" s="6">
@@ -6866,7 +6866,7 @@
       <c r="A113" s="1">
         <v>106</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="15" t="s">
         <v>206</v>
       </c>
       <c r="C113" s="6">
@@ -7103,7 +7103,7 @@
       <c r="A118" s="6">
         <v>111</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="15" t="s">
         <v>207</v>
       </c>
       <c r="C118" s="6">
@@ -7631,7 +7631,7 @@
       <c r="A130" s="6">
         <v>123</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="15" t="s">
         <v>208</v>
       </c>
       <c r="C130" s="6">
@@ -7827,7 +7827,7 @@
       <c r="A134" s="6">
         <v>127</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="15" t="s">
         <v>209</v>
       </c>
       <c r="C134" s="6">
@@ -7981,7 +7981,7 @@
       <c r="A137" s="1">
         <v>130</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="15" t="s">
         <v>210</v>
       </c>
       <c r="C137" s="6">
@@ -8135,7 +8135,7 @@
       <c r="A140" s="6">
         <v>133</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="15" t="s">
         <v>211</v>
       </c>
       <c r="C140" s="6">
@@ -8248,7 +8248,7 @@
       <c r="A142" s="6">
         <v>135</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="15" t="s">
         <v>212</v>
       </c>
       <c r="C142" s="6">
@@ -8444,7 +8444,7 @@
       <c r="A146" s="6">
         <v>139</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="15" t="s">
         <v>213</v>
       </c>
       <c r="C146" s="6">
@@ -8598,7 +8598,7 @@
       <c r="A149" s="1">
         <v>142</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="15" t="s">
         <v>214</v>
       </c>
       <c r="C149" s="6">
@@ -8620,7 +8620,7 @@
         <v>14</v>
       </c>
       <c r="I149" s="6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J149" s="15">
         <v>0</v>
@@ -8748,7 +8748,7 @@
       <c r="A152" s="6">
         <v>145</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B152" s="15" t="s">
         <v>215</v>
       </c>
       <c r="C152" s="6">
@@ -8902,7 +8902,7 @@
       <c r="A155" s="1">
         <v>148</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B155" s="15" t="s">
         <v>216</v>
       </c>
       <c r="C155" s="6">
@@ -9014,7 +9014,7 @@
       <c r="A157" s="1">
         <v>150</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B157" s="15" t="s">
         <v>217</v>
       </c>
       <c r="C157" s="6">
@@ -9168,7 +9168,7 @@
       <c r="A160" s="6">
         <v>153</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="15" t="s">
         <v>218</v>
       </c>
       <c r="C160" s="6">
@@ -9322,7 +9322,7 @@
       <c r="A163" s="1">
         <v>156</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="15" t="s">
         <v>219</v>
       </c>
       <c r="C163" s="2">
@@ -9434,7 +9434,7 @@
       <c r="A165" s="1">
         <v>158</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165" s="15" t="s">
         <v>220</v>
       </c>
       <c r="C165" s="2">
@@ -9588,7 +9588,7 @@
       <c r="A168" s="6">
         <v>161</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B168" s="15" t="s">
         <v>221</v>
       </c>
       <c r="C168" s="2">
@@ -9701,7 +9701,7 @@
       <c r="A170" s="6">
         <v>163</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="15" t="s">
         <v>222</v>
       </c>
       <c r="C170" s="2">
@@ -9814,7 +9814,7 @@
       <c r="A172" s="6">
         <v>165</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B172" s="15" t="s">
         <v>223</v>
       </c>
       <c r="C172" s="2">
@@ -9968,7 +9968,7 @@
       <c r="A175" s="1">
         <v>168</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B175" s="15" t="s">
         <v>224</v>
       </c>
       <c r="C175" s="2">
@@ -10205,7 +10205,7 @@
       <c r="A180" s="6">
         <v>173</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="15" t="s">
         <v>225</v>
       </c>
       <c r="C180" s="6">
@@ -10276,7 +10276,7 @@
       <c r="A181" s="1">
         <v>174</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B181" s="15" t="s">
         <v>226</v>
       </c>
       <c r="C181" s="6">
@@ -10430,7 +10430,7 @@
       <c r="A184" s="6">
         <v>177</v>
       </c>
-      <c r="B184" t="s">
+      <c r="B184" s="15" t="s">
         <v>227</v>
       </c>
       <c r="C184" s="6">
@@ -10626,7 +10626,7 @@
       <c r="A188" s="6">
         <v>181</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="15" t="s">
         <v>228</v>
       </c>
       <c r="C188" s="6">
@@ -10780,7 +10780,7 @@
       <c r="A191" s="1">
         <v>184</v>
       </c>
-      <c r="B191" t="s">
+      <c r="B191" s="15" t="s">
         <v>229</v>
       </c>
       <c r="C191" s="6">
@@ -10934,7 +10934,7 @@
       <c r="A194" s="6">
         <v>187</v>
       </c>
-      <c r="B194" t="s">
+      <c r="B194" s="15" t="s">
         <v>230</v>
       </c>
       <c r="C194" s="6">
@@ -11088,7 +11088,7 @@
       <c r="A197" s="1">
         <v>190</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B197" s="15" t="s">
         <v>231</v>
       </c>
       <c r="C197" s="6">
@@ -11242,7 +11242,7 @@
       <c r="A200" s="6">
         <v>193</v>
       </c>
-      <c r="B200" t="s">
+      <c r="B200" s="15" t="s">
         <v>232</v>
       </c>
       <c r="C200" s="2">
@@ -11355,7 +11355,7 @@
       <c r="A202" s="6">
         <v>195</v>
       </c>
-      <c r="B202" t="s">
+      <c r="B202" s="15" t="s">
         <v>233</v>
       </c>
       <c r="C202" s="2">
@@ -11468,7 +11468,7 @@
       <c r="A204" s="6">
         <v>197</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="15" t="s">
         <v>234</v>
       </c>
       <c r="C204" s="2">
@@ -11581,7 +11581,7 @@
       <c r="A206" s="6">
         <v>199</v>
       </c>
-      <c r="B206" t="s">
+      <c r="B206" s="15" t="s">
         <v>235</v>
       </c>
       <c r="C206" s="2">
@@ -11694,7 +11694,7 @@
       <c r="A208" s="6">
         <v>201</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B208" s="15" t="s">
         <v>236</v>
       </c>
       <c r="C208" s="2">
@@ -11807,7 +11807,7 @@
       <c r="A210" s="6">
         <v>203</v>
       </c>
-      <c r="B210" t="s">
+      <c r="B210" s="15" t="s">
         <v>237</v>
       </c>
       <c r="C210" s="2">
@@ -11961,7 +11961,7 @@
       <c r="A213" s="1">
         <v>206</v>
       </c>
-      <c r="B213" t="s">
+      <c r="B213" s="15" t="s">
         <v>238</v>
       </c>
       <c r="C213" s="2">
@@ -12073,7 +12073,7 @@
       <c r="A215" s="1">
         <v>208</v>
       </c>
-      <c r="B215" t="s">
+      <c r="B215" s="15" t="s">
         <v>239</v>
       </c>
       <c r="C215" s="2">
@@ -12227,7 +12227,7 @@
       <c r="A218" s="6">
         <v>211</v>
       </c>
-      <c r="B218" t="s">
+      <c r="B218" s="15" t="s">
         <v>240</v>
       </c>
       <c r="C218" s="6">
@@ -12423,7 +12423,7 @@
       <c r="A222" s="6">
         <v>215</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B222" s="15" t="s">
         <v>241</v>
       </c>
       <c r="C222" s="6">

</xml_diff>